<commit_message>
refactor: update sales dataframe
</commit_message>
<xml_diff>
--- a/Sales.xlsx
+++ b/Sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathalia/Projetos/managing-sales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D91AA62-11B8-9F48-9C02-7368F29CFDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B51F5B-3C87-1E46-AFD5-BEE82931EEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,8 +411,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="11">
-        <v>44470</v>
+        <v>44440</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>11</v>
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="11">
-        <v>44470</v>
+        <v>44440</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
@@ -561,7 +561,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="11">
-        <v>44470</v>
+        <v>44440</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>17</v>
@@ -578,7 +578,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="11">
-        <v>44471</v>
+        <v>44441</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>11</v>
@@ -595,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="11">
-        <v>44471</v>
+        <v>44441</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="11">
-        <v>44471</v>
+        <v>44441</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>17</v>
@@ -629,7 +629,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="11">
-        <v>44471</v>
+        <v>44441</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>11</v>
@@ -646,7 +646,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="11">
-        <v>44472</v>
+        <v>44442</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>11</v>
@@ -663,7 +663,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="11">
-        <v>44472</v>
+        <v>44442</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>11</v>
@@ -680,7 +680,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="11">
-        <v>44473</v>
+        <v>44443</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>17</v>
@@ -697,7 +697,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="11">
-        <v>44473</v>
+        <v>44443</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -714,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="11">
-        <v>44473</v>
+        <v>44443</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>

</xml_diff>